<commit_message>
Appointment table add in ABS
</commit_message>
<xml_diff>
--- a/docs/DoctorManagementSystem.xlsx
+++ b/docs/DoctorManagementSystem.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CarltonIT4\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
@@ -15,8 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -137,12 +132,6 @@
     <t>DateOfDischarge</t>
   </si>
   <si>
-    <t>DateOfVisit</t>
-  </si>
-  <si>
-    <t>FeeDeposited</t>
-  </si>
-  <si>
     <t>ItemId</t>
   </si>
   <si>
@@ -203,26 +192,89 @@
     <t>Department  -5</t>
   </si>
   <si>
-    <t>PatientDiagnosisIndoor  -6</t>
-  </si>
-  <si>
-    <t>PatientDiagnosisOutdoor   -7</t>
-  </si>
-  <si>
-    <t>ItemMasterIndoorPatient  -8</t>
-  </si>
-  <si>
-    <t>IndoorPatientBill    -9</t>
-  </si>
-  <si>
-    <t>MedicineMaster   -10</t>
+    <t>PatientIndoor  -6</t>
+  </si>
+  <si>
+    <t>AppoId</t>
+  </si>
+  <si>
+    <t>FkDepartmentId</t>
+  </si>
+  <si>
+    <t>FkDoctorId</t>
+  </si>
+  <si>
+    <t>SloltDate</t>
+  </si>
+  <si>
+    <t>SloltTimeStart</t>
+  </si>
+  <si>
+    <t>SloltTimeEnd</t>
+  </si>
+  <si>
+    <t>DocSlotID</t>
+  </si>
+  <si>
+    <t>fkDocSlotID</t>
+  </si>
+  <si>
+    <t>TimeSlotId</t>
+  </si>
+  <si>
+    <t>FkTimeSlotId</t>
+  </si>
+  <si>
+    <t>DoctorFee</t>
+  </si>
+  <si>
+    <t>ItemMasterIndoorPatient  -7</t>
+  </si>
+  <si>
+    <t>IndoorPatientBill    -8</t>
+  </si>
+  <si>
+    <t>MedicineMaster   -9</t>
+  </si>
+  <si>
+    <t>Appointment   -10</t>
+  </si>
+  <si>
+    <t>AppointmentSlot  -11</t>
+  </si>
+  <si>
+    <t>TimeSlot - 12</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>ItemPriceTotal</t>
+  </si>
+  <si>
+    <t>MedicinePriceTotal</t>
+  </si>
+  <si>
+    <t>TotalPrice</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>1. Appointment table will be used for Outdoor patient too.</t>
+  </si>
+  <si>
+    <t>DocLatitude</t>
+  </si>
+  <si>
+    <t>DocLongitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,7 +289,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +299,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCF9FFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,16 +327,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCF9FFF"/>
+      <color rgb="FFEAD5FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -539,439 +611,571 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C89"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>51</v>
-      </c>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>